<commit_message>
Update the building name of WER
</commit_message>
<xml_diff>
--- a/Mapping/unimelb_werribee_url.xlsx
+++ b/Mapping/unimelb_werribee_url.xlsx
@@ -16,16 +16,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
-    <t>Building name</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>url</t>
-  </si>
-  <si>
-    <t>WERRIBEE VETERINARY HOSPITAL</t>
+    <t>building_name</t>
+  </si>
+  <si>
+    <t>building_no</t>
+  </si>
+  <si>
+    <t>website:map</t>
+  </si>
+  <si>
+    <t>WERRIBEE BUILDING 411</t>
   </si>
   <si>
     <t>WERRIBEE PATHOLOGY BUILDING</t>
@@ -37,7 +37,7 @@
     <t>WERRIBEE LEARNING &amp; TEACHING BUILDING</t>
   </si>
   <si>
-    <t>WERRIBEE CAMPUS SERVICES WORKSHOP/STORE</t>
+    <t>WERRIBEE CAMPUS MANAGEMENT OFFICE</t>
   </si>
   <si>
     <t>WERRIBEE RESEARCH LABORATORY</t>

</xml_diff>